<commit_message>
known issues - exe3
</commit_message>
<xml_diff>
--- a/KnownIssues_ID1_ID2_.xlsx
+++ b/KnownIssues_ID1_ID2_.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lioro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lioro\Documents\Visual Studio 2015\Projects\check1\check1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nUGsX3qFFz0bxuM3tWqqJfJRUUGCpNwQD6oLnKZwRKNR37TfSXSY7seWZfweU7t+k7KvszATrKClwIJtlAYmoQ==" workbookSaltValue="kqfwAKTifn68EAoAQsB+5w==" workbookSpinCount="100000" lockStructure="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>ID 1:</t>
   </si>
@@ -169,7 +169,7 @@
     <t>Dor Galam</t>
   </si>
   <si>
-    <t>there is no Known issue</t>
+    <t>function calculate - switch cases for 3 operators - can't reduse number of cases,because we want a variaty of questions with 3 operators</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -684,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -741,22 +741,26 @@
       <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="G8" s="10" t="str">
         <f t="shared" ref="G8:G27" si="0">$H$7&amp;C8</f>
-        <v>Reproducibility</v>
+        <v>ReproducibilityCode</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" spans="2:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9">

</xml_diff>

<commit_message>
bullet - creature fix
</commit_message>
<xml_diff>
--- a/KnownIssues_ID1_ID2_.xlsx
+++ b/KnownIssues_ID1_ID2_.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lioro\Documents\Visual Studio 2015\Projects\check1\check1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lioro\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="nUGsX3qFFz0bxuM3tWqqJfJRUUGCpNwQD6oLnKZwRKNR37TfSXSY7seWZfweU7t+k7KvszATrKClwIJtlAYmoQ==" workbookSaltValue="kqfwAKTifn68EAoAQsB+5w==" workbookSpinCount="100000" lockStructure="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>ID 1:</t>
   </si>
@@ -169,7 +169,7 @@
     <t>Dor Galam</t>
   </si>
   <si>
-    <t>function calculate - switch cases for 3 operators - can't reduse number of cases,because we want a variaty of questions with 3 operators</t>
+    <t>there is no Known issue</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="B2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -684,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -741,26 +741,22 @@
       <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="10" t="str">
         <f t="shared" ref="G8:G27" si="0">$H$7&amp;C8</f>
-        <v>ReproducibilityCode</v>
+        <v>Reproducibility</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="K8" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="2:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9">

</xml_diff>